<commit_message>
corregir diccionario de datos
</commit_message>
<xml_diff>
--- a/Documentación/Diccionario de datos.xlsx
+++ b/Documentación/Diccionario de datos.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
   <si>
     <r>
       <t xml:space="preserve">Nombre de archivo: </t>
@@ -59,6 +59,18 @@
     </r>
   </si>
   <si>
+    <t>Campo</t>
+  </si>
+  <si>
+    <t>Tamaño</t>
+  </si>
+  <si>
+    <t>Tipo de dato</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Nombre de archivo: </t>
     </r>
@@ -85,16 +97,13 @@
     </r>
   </si>
   <si>
-    <t>Campo</t>
-  </si>
-  <si>
-    <t>Tamaño</t>
-  </si>
-  <si>
-    <t>Tipo de dato</t>
-  </si>
-  <si>
-    <t>Descripcion</t>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>numerico</t>
+  </si>
+  <si>
+    <t>Telefono perteneciente al trabajador</t>
   </si>
   <si>
     <r>
@@ -110,15 +119,6 @@
     </r>
   </si>
   <si>
-    <t>telefono</t>
-  </si>
-  <si>
-    <t>numerico</t>
-  </si>
-  <si>
-    <t>Telefono perteneciente al trabajador</t>
-  </si>
-  <si>
     <t>foto-perfil</t>
   </si>
   <si>
@@ -128,16 +128,22 @@
     <t>ruta/nombre hacia la Foto que identifique al trabajador</t>
   </si>
   <si>
+    <t>foto-documento</t>
+  </si>
+  <si>
+    <t>ruta/nombre hacia la imagen del documento de identidad del trabajador</t>
+  </si>
+  <si>
     <t>id-labor</t>
   </si>
   <si>
     <t xml:space="preserve">Numero de identificacion de la labor </t>
   </si>
   <si>
-    <t>foto-documento</t>
-  </si>
-  <si>
-    <t>ruta/nombre hacia la imagen del documento de identidad del trabajador</t>
+    <t xml:space="preserve">nombre  </t>
+  </si>
+  <si>
+    <t>Nombre del trabajador</t>
   </si>
   <si>
     <t>nombre-labor</t>
@@ -146,10 +152,10 @@
     <t>Nombre que identifica la labor</t>
   </si>
   <si>
-    <t xml:space="preserve">nombre  </t>
-  </si>
-  <si>
-    <t>Nombre del trabajador</t>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Cedula de ciudadania del trabajador</t>
   </si>
   <si>
     <t>tipo-labor</t>
@@ -158,10 +164,13 @@
     <t>clasificación de la labor(domestica,educativa,social,etc)</t>
   </si>
   <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Cedula de ciudadania del trabajador</t>
+    <t>direccion</t>
+  </si>
+  <si>
+    <t>geometrico</t>
+  </si>
+  <si>
+    <t>coordenadas de la Direccion de residencia del trabajador</t>
   </si>
   <si>
     <r>
@@ -190,15 +199,6 @@
     </r>
   </si>
   <si>
-    <t>direccion</t>
-  </si>
-  <si>
-    <t>geometrico</t>
-  </si>
-  <si>
-    <t>coordenadas de la Direccion de residencia del trabajador</t>
-  </si>
-  <si>
     <t>disponibilidad</t>
   </si>
   <si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>Numero promedio de estrellas del trabajador</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>password para ingresar a la plataforma</t>
   </si>
   <si>
     <r>
@@ -286,12 +292,6 @@
     <t>trabajador-telefono</t>
   </si>
   <si>
-    <t>unidad-labor</t>
-  </si>
-  <si>
-    <t>Precio por hora que cobra el trabajador por su labor</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Nombre de archivo: </t>
     </r>
@@ -318,6 +318,25 @@
     </r>
   </si>
   <si>
+    <t>unidad-labor</t>
+  </si>
+  <si>
+    <t>Precio por hora que cobra el trabajador por su labor</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Descripcion: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Contiene la informacion personal del usuario que utilizara la aplicación</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Relaciones: </t>
     </r>
@@ -344,23 +363,13 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Descripcion: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Contiene la informacion personal del usuario que utilizara la aplicación</t>
-    </r>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
     <t>Nombre del usuario</t>
+  </si>
+  <si>
+    <t>coordenadass de la Direccion de residencia del usuario</t>
   </si>
   <si>
     <r>
@@ -390,7 +399,10 @@
     </r>
   </si>
   <si>
-    <t>coordenadass de la Direccion de residencia del usuario</t>
+    <t>foto-recibo-servicios</t>
+  </si>
+  <si>
+    <t>ruta/nombre hacia la foto que verifique la residencia del usuario</t>
   </si>
   <si>
     <r>
@@ -404,12 +416,6 @@
       </rPr>
       <t>Contiene la informacion del trabajador y usuario, ademas de el precio y calificacion que dio este ultimo al trabajador</t>
     </r>
-  </si>
-  <si>
-    <t>foto-recibo-servicios</t>
-  </si>
-  <si>
-    <t>ruta/nombre hacia la foto que verifique la residencia del usuario</t>
   </si>
   <si>
     <t>e-mail</t>
@@ -507,7 +513,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -521,12 +527,11 @@
     </font>
     <font/>
     <font>
+      <b/>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <sz val="11.0"/>
       <color theme="1"/>
     </font>
@@ -537,10 +542,15 @@
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -655,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -670,33 +680,33 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -712,14 +722,17 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -731,16 +744,25 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -980,47 +1002,61 @@
     <col customWidth="1" min="11" max="26" width="9.38"/>
   </cols>
   <sheetData>
+    <row r="3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
     <row r="4">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5">
-      <c r="B5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J5" s="4"/>
     </row>
     <row r="6">
-      <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>8</v>
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1028,142 +1064,142 @@
     </row>
     <row r="7">
       <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="8">
-        <v>10.0</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="10">
+        <v>100.0</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="J7" s="12" t="s">
         <v>6</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="11">
+        <v>16</v>
+      </c>
+      <c r="C8" s="10">
         <v>100.0</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="12">
+      <c r="E8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="14">
         <v>10.0</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>11</v>
+      <c r="I8" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="11">
-        <v>100.0</v>
-      </c>
-      <c r="D9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="10">
+        <v>50.0</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="11">
+      <c r="E9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="16">
         <v>50.0</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="11">
+        <v>24</v>
+      </c>
+      <c r="C10" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="16">
         <v>50.0</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="I10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="17">
-        <v>50.0</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="J10" s="18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" s="8">
-        <v>10.0</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>27</v>
+        <v>20.0</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="21" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J11" s="22"/>
     </row>
     <row r="12">
       <c r="B12" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12" s="8">
-        <v>20.0</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>32</v>
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="24"/>
@@ -1172,51 +1208,51 @@
     </row>
     <row r="13">
       <c r="B13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1.0</v>
+        <v>36</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="26" t="s">
+      <c r="B14" s="26" t="s">
         <v>39</v>
+      </c>
+      <c r="C14" s="27">
+        <v>50.0</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>41</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J14" s="4"/>
     </row>
     <row r="15">
       <c r="B15" s="19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" s="22"/>
       <c r="G15" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1227,160 +1263,172 @@
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="E16" s="25"/>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="J16" s="12" t="s">
         <v>6</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="G17" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="12">
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="G17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="14">
         <v>10.0</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>11</v>
+      <c r="I17" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
-      <c r="G18" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" s="12">
+      <c r="G18" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="14">
         <v>10.0</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="15" t="s">
         <v>11</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="19">
-      <c r="G19" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="30">
+      <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="G19" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="31">
         <v>20.0</v>
       </c>
-      <c r="I19" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="31" t="s">
-        <v>46</v>
+      <c r="I19" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="32" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="1" t="s">
-        <v>47</v>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="4"/>
-      <c r="G20" s="32" t="s">
-        <v>49</v>
+      <c r="G20" s="33" t="s">
+        <v>52</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="21" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J20" s="22"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="4"/>
+      <c r="B21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="G21" s="23"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
       <c r="J21" s="25"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>8</v>
+      <c r="B22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="8">
-        <v>10.0</v>
+        <v>54</v>
+      </c>
+      <c r="C23" s="10">
+        <v>50.0</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" ht="15.0" customHeight="1">
       <c r="B24" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="26" t="s">
-        <v>54</v>
+        <v>28</v>
+      </c>
+      <c r="C24" s="8">
+        <v>20.0</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="B25" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="8">
-        <v>20.0</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="32" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="C25" s="10">
+        <v>100.0</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
@@ -1388,16 +1436,16 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="B26" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="11">
-        <v>100.0</v>
-      </c>
-      <c r="D26" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="10">
+        <v>50.0</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>59</v>
+      <c r="E26" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="G26" s="23"/>
       <c r="H26" s="24"/>
@@ -1406,76 +1454,76 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="B27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="11">
-        <v>50.0</v>
+        <v>64</v>
+      </c>
+      <c r="C27" s="10">
+        <v>20.0</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="34" t="s">
+      <c r="J27" s="34" t="s">
         <v>6</v>
-      </c>
-      <c r="I27" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27" s="33" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="11">
-        <v>20.0</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="B28" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="37">
+        <v>50.0</v>
+      </c>
+      <c r="D28" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>64</v>
+      <c r="E28" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="H28" s="15">
         <v>10.0</v>
       </c>
-      <c r="I28" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>65</v>
+      <c r="I28" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="B29" s="19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E29" s="22"/>
-      <c r="G29" s="14" t="s">
-        <v>16</v>
+      <c r="G29" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="H29" s="15">
         <v>10.0</v>
       </c>
-      <c r="I29" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>68</v>
+      <c r="I29" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -1483,54 +1531,54 @@
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
       <c r="E30" s="25"/>
-      <c r="G30" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H30" s="35">
+      <c r="G30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="39">
         <v>10.0</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="G31" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="H31" s="35">
+      <c r="G31" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" s="39">
         <v>10.0</v>
       </c>
-      <c r="I31" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>70</v>
+      <c r="I31" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="G32" s="14" t="s">
-        <v>71</v>
+      <c r="G32" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="H32" s="15">
         <v>1.0</v>
       </c>
-      <c r="I32" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" s="14" t="s">
-        <v>72</v>
+      <c r="I32" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="G33" s="32" t="s">
-        <v>73</v>
+      <c r="G33" s="33" t="s">
+        <v>75</v>
       </c>
       <c r="H33" s="20"/>
-      <c r="I33" s="36" t="s">
-        <v>74</v>
+      <c r="I33" s="40" t="s">
+        <v>76</v>
       </c>
       <c r="J33" s="22"/>
     </row>
@@ -2508,31 +2556,31 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="D29:E30"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="G6:J6"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="D29:E30"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="G25:J26"/>
     <mergeCell ref="G33:H34"/>
     <mergeCell ref="I33:J34"/>
+    <mergeCell ref="G11:H12"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:J15"/>
     <mergeCell ref="G20:H21"/>
     <mergeCell ref="I20:J21"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="D20:E20"/>
     <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="I11:J12"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>